<commit_message>
Updated the sensor box bill of materials file to the latest version on google drive
Had a few out of date parts that were sent to Dr mueller for replacement orders and some parts that were added during the prototyping process.
</commit_message>
<xml_diff>
--- a/BOM and Production hours estimate/Sensor box project bill of materials.xlsx
+++ b/BOM and Production hours estimate/Sensor box project bill of materials.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
   <si>
     <t>Part Name</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Ordered 2/11/2025</t>
+  </si>
+  <si>
+    <t>Corrected parts  05/24/2025</t>
   </si>
   <si>
     <t>SEN0232: Noise Sensor</t>
@@ -218,10 +221,16 @@
     <t>https://www.digikey.com/en/products/detail/raf-electronic-hardware/4011-440-AL/9834457</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/raf-electronic-hardware/1690-440-AL/11486834</t>
+  </si>
+  <si>
     <t>Hex nut 1/4 stainless steel 4-40</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/b-f-fastener-supply/HNSS440/274935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not needed </t>
   </si>
   <si>
     <t>Passivated 18-8 Stainless Steel Pan Head Phillips Screw
@@ -307,6 +316,21 @@
   </si>
   <si>
     <t xml:space="preserve">Isolating washers </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://www.mcmaster.com/90295A359-90295A059/-</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> 5 packs </t>
+    </r>
   </si>
   <si>
     <t>Gland</t>
@@ -359,7 +383,31 @@
     <t>PCB</t>
   </si>
   <si>
+    <t>Silicone</t>
+  </si>
+  <si>
     <t>https://www.amazon.com/GE-Advanced-Silicone-Kitchen-Bathroom/dp/B0C448QB1K/ref=sr_1_1?crid=31J1AYIR1NSCV&amp;dib=eyJ2IjoiMSJ9.wKigtWz-Huf-K6CrM-u3J-xtQcoeCvRIT1oTpQcPdx4ixfVnhKof58xRBggoTry6jUssNOdNY8GJJEqFS4A_WkSD7ZCdjnzxIEp7UEYVduAlcD2jQYfSFNCZKjr5OUwmr-zVEavJTqCJUO9v_o7XaDRMYfjH_MjOJZ8I7UZjlSpXqWXas0mAlpkafdDFFS1m6FNpL2Dz1WbPaQE__qLeVzfVdrtQgWsPJgwOQ49jCys.pTFp8Gwb2tL2_7Ts08uhvkfCyWV-BhgAFjvbQ5aVt3M&amp;dib_tag=se&amp;keywords=silicone&amp;qid=1739568697&amp;sprefix=silicone%2Caps%2C123&amp;sr=8-1&amp;th=1</t>
+  </si>
+  <si>
+    <t>Loctite</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://www.mcmaster.com/92855A401/-</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> 12 packs</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">M4 </t>
   </si>
   <si>
     <t>Total</t>
@@ -830,7 +878,9 @@
     <col customWidth="1" min="3" max="3" width="24.38"/>
     <col customWidth="1" min="4" max="4" width="17.25"/>
     <col customWidth="1" min="6" max="6" width="60.5"/>
-    <col customWidth="1" min="7" max="7" width="19.63"/>
+    <col customWidth="1" min="7" max="7" width="17.13"/>
+    <col customWidth="1" min="8" max="8" width="99.5"/>
+    <col customWidth="1" min="9" max="9" width="67.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -855,10 +905,14 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -869,7 +923,7 @@
         <v>1.0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="7">
         <v>50.0</v>
@@ -877,7 +931,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -888,7 +942,7 @@
         <v>1.0</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G3" s="7">
         <v>50.0</v>
@@ -896,7 +950,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -907,7 +961,7 @@
         <v>1.0</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" s="7">
         <v>50.0</v>
@@ -915,7 +969,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="9"/>
@@ -926,7 +980,7 @@
         <v>1.0</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="7">
         <v>50.0</v>
@@ -934,7 +988,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -945,15 +999,15 @@
         <v>1.0</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -964,7 +1018,7 @@
         <v>1.0</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G7" s="7">
         <v>55.0</v>
@@ -972,7 +1026,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="9"/>
@@ -983,7 +1037,7 @@
         <v>1.0</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="7">
         <v>50.0</v>
@@ -991,7 +1045,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="9"/>
@@ -1002,15 +1056,15 @@
         <v>1.0</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -1021,7 +1075,7 @@
         <v>1.0</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10" s="7">
         <v>200.0</v>
@@ -1029,7 +1083,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -1040,7 +1094,7 @@
         <v>1.0</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G11" s="7">
         <v>53.0</v>
@@ -1048,10 +1102,10 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="3">
@@ -1061,7 +1115,7 @@
         <v>1.0</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G12" s="7">
         <v>26.0</v>
@@ -1069,7 +1123,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1080,7 +1134,7 @@
         <v>2.0</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G13" s="7">
         <v>52.0</v>
@@ -1088,7 +1142,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -1099,18 +1153,18 @@
         <v>2.0</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -1121,7 +1175,7 @@
         <v>1.0</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G15" s="7">
         <v>26.0</v>
@@ -1129,7 +1183,7 @@
     </row>
     <row r="16">
       <c r="A16" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="4"/>
@@ -1140,15 +1194,15 @@
         <v>4.0</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="4"/>
@@ -1159,15 +1213,15 @@
         <v>11.0</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="4"/>
@@ -1178,15 +1232,15 @@
         <v>4.0</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1197,15 +1251,15 @@
         <v>4.0</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1216,7 +1270,7 @@
         <v>1.0</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G20" s="7">
         <v>250.0</v>
@@ -1224,7 +1278,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1235,18 +1289,18 @@
         <v>39.0</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -1257,7 +1311,7 @@
         <v>1.0</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G22" s="7">
         <v>50.0</v>
@@ -1265,7 +1319,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1276,7 +1330,7 @@
         <v>1.0</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G23" s="7">
         <v>55.0</v>
@@ -1284,7 +1338,7 @@
     </row>
     <row r="24">
       <c r="A24" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1295,7 +1349,7 @@
         <v>1.0</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G24" s="7">
         <v>55.0</v>
@@ -1303,7 +1357,7 @@
     </row>
     <row r="25">
       <c r="A25" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
@@ -1314,7 +1368,7 @@
         <v>1.0</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G25" s="7">
         <v>55.0</v>
@@ -1322,7 +1376,7 @@
     </row>
     <row r="26">
       <c r="A26" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="4"/>
@@ -1333,15 +1387,18 @@
         <v>4.0</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G26" s="7">
         <v>240.0</v>
       </c>
+      <c r="I26" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="4"/>
@@ -1352,18 +1409,21 @@
         <v>4.0</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G27" s="7">
         <v>200.0</v>
       </c>
+      <c r="I27" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="19">
@@ -1373,15 +1433,15 @@
         <v>4.0</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="4"/>
@@ -1392,15 +1452,15 @@
         <v>3.0</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="4"/>
@@ -1411,15 +1471,15 @@
         <v>3.0</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="4"/>
@@ -1430,15 +1490,15 @@
         <v>3.0</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="4"/>
@@ -1449,15 +1509,15 @@
         <v>3.0</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="4"/>
@@ -1468,7 +1528,7 @@
         <v>1.0</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G33" s="7">
         <v>50.0</v>
@@ -1476,7 +1536,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="4"/>
@@ -1487,7 +1547,7 @@
         <v>1.0</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G34" s="7">
         <v>50.0</v>
@@ -1495,7 +1555,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="4"/>
@@ -1506,7 +1566,7 @@
         <v>1.0</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G35" s="7">
         <v>50.0</v>
@@ -1514,7 +1574,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B36" s="19"/>
       <c r="C36" s="9"/>
@@ -1525,18 +1585,18 @@
         <v>1.0</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="4"/>
@@ -1547,7 +1607,7 @@
         <v>4.0</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G37" s="7">
         <v>220.0</v>
@@ -1555,7 +1615,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="4"/>
@@ -1566,15 +1626,15 @@
         <v>3.0</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="4"/>
@@ -1585,25 +1645,28 @@
         <v>3.0</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="18" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="4"/>
       <c r="D40" s="23"/>
       <c r="E40" s="24"/>
       <c r="G40" s="25"/>
+      <c r="I40" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="4"/>
@@ -1614,7 +1677,7 @@
         <v>1.0</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G41" s="7">
         <v>55.0</v>
@@ -1622,10 +1685,10 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="7">
@@ -1635,18 +1698,18 @@
         <v>30.0</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G42" s="25"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="4"/>
       <c r="D43" s="7" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E43" s="7">
         <v>2.0</v>
@@ -1655,10 +1718,10 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="19">
@@ -1668,7 +1731,7 @@
         <v>6.0</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G44" s="7">
         <v>4.0</v>
@@ -1676,13 +1739,13 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C45" s="26"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B46" s="27"/>
       <c r="D46" s="28">
@@ -1692,12 +1755,12 @@
         <v>1.0</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B47" s="27"/>
       <c r="D47" s="28">
@@ -1709,7 +1772,9 @@
       <c r="F47" s="7"/>
     </row>
     <row r="48">
-      <c r="A48" s="2"/>
+      <c r="A48" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B48" s="27"/>
       <c r="D48" s="28">
         <v>7.61</v>
@@ -1718,39 +1783,56 @@
         <v>1.0</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2"/>
+      <c r="A49" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="B49" s="27"/>
       <c r="D49" s="27"/>
+      <c r="I49" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="D50" s="30">
-        <f>SUM(D2:D49)</f>
+        <v>120</v>
+      </c>
+      <c r="B50" s="27"/>
+      <c r="D50" s="27"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="2"/>
+      <c r="B51" s="27"/>
+      <c r="D51" s="27"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="D52" s="30">
+        <f>SUM(D2:D51)</f>
         <v>481.594</v>
       </c>
     </row>
-    <row r="54">
-      <c r="B54" s="31" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
     <row r="56">
-      <c r="B56" s="4" t="s">
-        <v>117</v>
+      <c r="B56" s="31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1782,26 +1864,29 @@
     <hyperlink r:id="rId25" ref="F24"/>
     <hyperlink r:id="rId26" ref="F25"/>
     <hyperlink r:id="rId27" ref="F26"/>
-    <hyperlink r:id="rId28" ref="F27"/>
-    <hyperlink r:id="rId29" ref="F28"/>
-    <hyperlink r:id="rId30" ref="F29"/>
-    <hyperlink r:id="rId31" ref="F30"/>
-    <hyperlink r:id="rId32" ref="F31"/>
-    <hyperlink r:id="rId33" ref="F32"/>
-    <hyperlink r:id="rId34" ref="F33"/>
-    <hyperlink r:id="rId35" ref="F34"/>
-    <hyperlink r:id="rId36" ref="F35"/>
-    <hyperlink r:id="rId37" ref="F36"/>
-    <hyperlink r:id="rId38" ref="H36"/>
-    <hyperlink r:id="rId39" ref="F37"/>
-    <hyperlink r:id="rId40" ref="F38"/>
-    <hyperlink r:id="rId41" ref="F39"/>
-    <hyperlink r:id="rId42" ref="F41"/>
-    <hyperlink r:id="rId43" ref="F42"/>
-    <hyperlink r:id="rId44" ref="F44"/>
-    <hyperlink r:id="rId45" ref="F46"/>
-    <hyperlink r:id="rId46" ref="F48"/>
+    <hyperlink r:id="rId28" ref="I26"/>
+    <hyperlink r:id="rId29" ref="F27"/>
+    <hyperlink r:id="rId30" ref="F28"/>
+    <hyperlink r:id="rId31" ref="F29"/>
+    <hyperlink r:id="rId32" ref="F30"/>
+    <hyperlink r:id="rId33" ref="F31"/>
+    <hyperlink r:id="rId34" ref="F32"/>
+    <hyperlink r:id="rId35" ref="F33"/>
+    <hyperlink r:id="rId36" ref="F34"/>
+    <hyperlink r:id="rId37" ref="F35"/>
+    <hyperlink r:id="rId38" ref="F36"/>
+    <hyperlink r:id="rId39" ref="H36"/>
+    <hyperlink r:id="rId40" ref="F37"/>
+    <hyperlink r:id="rId41" ref="F38"/>
+    <hyperlink r:id="rId42" ref="F39"/>
+    <hyperlink r:id="rId43" ref="I40"/>
+    <hyperlink r:id="rId44" ref="F41"/>
+    <hyperlink r:id="rId45" ref="F42"/>
+    <hyperlink r:id="rId46" ref="F44"/>
+    <hyperlink r:id="rId47" ref="F46"/>
+    <hyperlink r:id="rId48" ref="F48"/>
+    <hyperlink r:id="rId49" ref="I49"/>
   </hyperlinks>
-  <drawing r:id="rId47"/>
+  <drawing r:id="rId50"/>
 </worksheet>
 </file>
</xml_diff>